<commit_message>
duplication of Jon's paper
</commit_message>
<xml_diff>
--- a/gui_key.xlsx
+++ b/gui_key.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Postdoc_UNC\CAL_water_price_index\CALFEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="8856" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="3953" yWindow="893" windowWidth="16200" windowHeight="12337" tabRatio="727" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_data" sheetId="7" r:id="rId1"/>
@@ -1799,7 +1800,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1824,7 +1825,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1840,6 +1841,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1918,25 +1931,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2216,43 +2224,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.21875" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="36.19921875" customWidth="1"/>
+    <col min="2" max="2" width="46.1328125" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>571</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="10" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>334</v>
       </c>
@@ -2272,7 +2280,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>335</v>
       </c>
@@ -2292,7 +2300,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>327</v>
       </c>
@@ -2312,7 +2320,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>336</v>
       </c>
@@ -2332,7 +2340,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>337</v>
       </c>
@@ -2352,7 +2360,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>495</v>
       </c>
@@ -2372,7 +2380,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>525</v>
       </c>
@@ -2392,7 +2400,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>529</v>
       </c>
@@ -2412,7 +2420,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>531</v>
       </c>
@@ -2432,7 +2440,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>533</v>
       </c>
@@ -2452,7 +2460,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>535</v>
       </c>
@@ -2472,7 +2480,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>537</v>
       </c>
@@ -2492,7 +2500,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>539</v>
       </c>
@@ -2512,7 +2520,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>541</v>
       </c>
@@ -2532,7 +2540,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>543</v>
       </c>
@@ -2552,7 +2560,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>545</v>
       </c>
@@ -2572,7 +2580,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>547</v>
       </c>
@@ -2592,7 +2600,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>549</v>
       </c>
@@ -2612,7 +2620,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>551</v>
       </c>
@@ -2632,7 +2640,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>553</v>
       </c>
@@ -2652,7 +2660,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>555</v>
       </c>
@@ -2672,7 +2680,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>557</v>
       </c>
@@ -2692,7 +2700,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>559</v>
       </c>
@@ -2712,7 +2720,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>561</v>
       </c>
@@ -2732,7 +2740,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>563</v>
       </c>
@@ -2752,7 +2760,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>565</v>
       </c>
@@ -2772,7 +2780,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>567</v>
       </c>
@@ -2792,7 +2800,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>569</v>
       </c>
@@ -2819,108 +2827,83 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="38.21875" customWidth="1"/>
+    <col min="3" max="3" width="20.1328125" customWidth="1"/>
+    <col min="5" max="5" width="38.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>262</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>261</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>260</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:C27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C27">
     <sortCondition ref="C2:C27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2928,24 +2911,24 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" customWidth="1"/>
+    <col min="2" max="2" width="49.46484375" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="38.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.1328125" customWidth="1"/>
+    <col min="7" max="7" width="38.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -2955,14 +2938,14 @@
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="5" t="s">
         <v>496</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>474</v>
       </c>
@@ -2972,14 +2955,14 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>475</v>
       </c>
@@ -2989,14 +2972,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>494</v>
       </c>
@@ -3006,14 +2989,14 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>476</v>
       </c>
@@ -3023,14 +3006,14 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>477</v>
       </c>
@@ -3040,99 +3023,99 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>478</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>507</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>479</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>506</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>480</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" t="s">
         <v>508</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="14">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>481</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" t="s">
         <v>509</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>482</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" t="s">
         <v>510</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14">
-        <v>1</v>
-      </c>
-      <c r="E11" s="14" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>483</v>
       </c>
@@ -3142,14 +3125,14 @@
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>484</v>
       </c>
@@ -3159,14 +3142,14 @@
       <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>485</v>
       </c>
@@ -3176,14 +3159,14 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>486</v>
       </c>
@@ -3193,14 +3176,14 @@
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>487</v>
       </c>
@@ -3210,14 +3193,14 @@
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>488</v>
       </c>
@@ -3227,14 +3210,14 @@
       <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>489</v>
       </c>
@@ -3244,14 +3227,14 @@
       <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>490</v>
       </c>
@@ -3261,14 +3244,14 @@
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>491</v>
       </c>
@@ -3278,14 +3261,14 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>492</v>
       </c>
@@ -3295,14 +3278,14 @@
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>493</v>
       </c>
@@ -3312,7 +3295,7 @@
       <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
@@ -3325,22 +3308,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.46484375" customWidth="1"/>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3351,7 +3334,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>468</v>
       </c>
@@ -3362,7 +3345,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>183</v>
       </c>
@@ -3373,7 +3356,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -3384,7 +3367,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>465</v>
       </c>
@@ -3395,7 +3378,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>462</v>
       </c>
@@ -3406,7 +3389,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -3417,7 +3400,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -3428,7 +3411,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>180</v>
       </c>
@@ -3439,7 +3422,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>456</v>
       </c>
@@ -3450,7 +3433,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>459</v>
       </c>
@@ -3461,7 +3444,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>184</v>
       </c>
@@ -3472,39 +3455,30 @@
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>580</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>581</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" t="s">
         <v>582</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>583</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" t="s">
         <v>584</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:C21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C21">
     <sortCondition ref="C2:C21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3513,23 +3487,23 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.46484375" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -3539,14 +3513,14 @@
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="5" t="s">
         <v>496</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>473</v>
       </c>
@@ -3556,84 +3530,12 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3642,231 +3544,186 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:B15"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3875,24 +3732,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B9" sqref="B9"/>
+      <selection pane="topRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.53125" customWidth="1"/>
+    <col min="2" max="2" width="30.19921875" customWidth="1"/>
     <col min="3" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -3909,7 +3766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3926,7 +3783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3943,7 +3800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3960,7 +3817,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3977,7 +3834,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -3994,7 +3851,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>279</v>
       </c>
@@ -4011,7 +3868,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>191</v>
       </c>
@@ -4028,7 +3885,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -4045,7 +3902,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -4062,7 +3919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4079,7 +3936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -4096,59 +3953,57 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" t="s">
         <v>353</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="14">
-        <v>1</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>367</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" t="s">
         <v>368</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="14" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>369</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" t="s">
         <v>370</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="14">
-        <v>1</v>
-      </c>
-      <c r="E15" s="14" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4156,85 +4011,70 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.46484375" customWidth="1"/>
+    <col min="2" max="2" width="12.86328125" customWidth="1"/>
+    <col min="3" max="3" width="19.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.46484375" customWidth="1"/>
+    <col min="2" max="2" width="37.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.86328125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -4244,48 +4084,48 @@
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="5" t="s">
         <v>496</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>382</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>572</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>381</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" t="s">
         <v>573</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-      <c r="E3" s="14" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>380</v>
       </c>
@@ -4295,14 +4135,14 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -4312,14 +4152,14 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -4329,14 +4169,14 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -4346,66 +4186,66 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" t="s">
         <v>377</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="14">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" t="s">
         <v>376</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="14">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" t="s">
         <v>378</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>275</v>
       </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -4415,14 +4255,14 @@
       <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>267</v>
       </c>
@@ -4432,14 +4272,14 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>266</v>
       </c>
@@ -4449,31 +4289,31 @@
       <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -4483,14 +4323,14 @@
       <c r="C15" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -4500,14 +4340,14 @@
       <c r="C16" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>385</v>
       </c>
@@ -4517,7 +4357,7 @@
       <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
@@ -4525,7 +4365,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
     <sortCondition ref="B2:B17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4534,384 +4374,337 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="4" max="4" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>433</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>286</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>287</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>436</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>434</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" t="s">
         <v>284</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" t="s">
         <v>285</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" t="s">
         <v>437</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
         <v>394</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" t="s">
         <v>291</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" t="s">
         <v>438</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" t="s">
         <v>290</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" t="s">
         <v>439</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" t="s">
         <v>289</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="36.1328125" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>500</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="11">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>389</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>390</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>391</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="11">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>392</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="11">
-        <v>1</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>194</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>393</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="11">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4919,666 +4712,652 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E24" sqref="E23:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.53125" customWidth="1"/>
+    <col min="4" max="4" width="9.796875" customWidth="1"/>
+    <col min="5" max="5" width="11.53125" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>249</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>259</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>205</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>208</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>238</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>454</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>219</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>455</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>254</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>239</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" t="s">
         <v>234</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>167</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>251</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" t="s">
         <v>218</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" t="s">
         <v>210</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" t="s">
         <v>224</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>165</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" t="s">
         <v>250</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" t="s">
         <v>225</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" t="s">
         <v>226</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" t="s">
         <v>211</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" t="s">
         <v>227</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" t="s">
         <v>241</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" t="s">
         <v>220</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" t="s">
         <v>253</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" t="s">
         <v>222</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" t="s">
         <v>228</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" t="s">
         <v>212</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>168</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" t="s">
         <v>252</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>128</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" t="s">
         <v>229</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" t="s">
         <v>213</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" t="s">
         <v>230</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" t="s">
         <v>237</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" t="s">
         <v>236</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" t="s">
         <v>231</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" t="s">
         <v>232</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>110</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" t="s">
         <v>214</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>111</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" t="s">
         <v>215</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>133</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" t="s">
         <v>470</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" t="s">
         <v>472</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>112</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" t="s">
         <v>216</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" t="s">
         <v>240</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" t="s">
         <v>217</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" t="s">
         <v>247</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>152</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" t="s">
         <v>245</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" t="s">
         <v>246</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>151</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" t="s">
         <v>244</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" t="s">
         <v>243</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>160</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" t="s">
         <v>248</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="8" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>149</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" t="s">
         <v>242</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sortState ref="A2:C78">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C78">
     <sortCondition ref="C2:C78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5586,26 +5365,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" customWidth="1"/>
+    <col min="2" max="2" width="55.53125" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.53125" customWidth="1"/>
+    <col min="6" max="6" width="9.796875" customWidth="1"/>
+    <col min="7" max="7" width="11.53125" customWidth="1"/>
+    <col min="8" max="8" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -5615,14 +5394,14 @@
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="5" t="s">
         <v>496</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>300</v>
       </c>
@@ -5632,15 +5411,15 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
         <v>301</v>
       </c>
       <c r="B3" t="s">
@@ -5649,15 +5428,15 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="12" t="s">
         <v>302</v>
       </c>
       <c r="B4" t="s">
@@ -5666,15 +5445,15 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="12" t="s">
         <v>303</v>
       </c>
       <c r="B5" t="s">
@@ -5683,15 +5462,15 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="12" t="s">
         <v>304</v>
       </c>
       <c r="B6" t="s">
@@ -5700,15 +5479,15 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="12" t="s">
         <v>306</v>
       </c>
       <c r="B7" t="s">
@@ -5717,116 +5496,116 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" t="s">
         <v>507</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="14">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" t="s">
         <v>508</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="14">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" t="s">
         <v>509</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>473</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" t="s">
         <v>510</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14">
-        <v>1</v>
-      </c>
-      <c r="E11" s="14" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" t="s">
         <v>511</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="14">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" t="s">
         <v>512</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="14">
-        <v>1</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -5836,14 +5615,14 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -5853,14 +5632,14 @@
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -5870,14 +5649,14 @@
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -5887,14 +5666,14 @@
       <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -5904,14 +5683,14 @@
       <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>187</v>
       </c>
@@ -5921,15 +5700,15 @@
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
         <v>197</v>
       </c>
       <c r="B20" t="s">
@@ -5938,15 +5717,15 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
         <v>199</v>
       </c>
       <c r="B21" t="s">
@@ -5955,14 +5734,14 @@
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>314</v>
       </c>
@@ -5972,7 +5751,7 @@
       <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
@@ -5981,5 +5760,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
time horizon expansion to 28 years
</commit_message>
<xml_diff>
--- a/gui_key.xlsx
+++ b/gui_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Postdoc_UNC\CAL_water_price_index\CALFEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/danli_ad_unc_edu/Documents/github/CALFEWS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF00F5CC-4515-4ADF-B944-3C30D6D19FBD}"/>
   <bookViews>
-    <workbookView xWindow="3953" yWindow="893" windowWidth="16200" windowHeight="12337" tabRatio="727" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23676" yWindow="1944" windowWidth="18816" windowHeight="12900" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_data" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="589">
   <si>
     <t>Object List</t>
   </si>
@@ -1795,13 +1795,22 @@
   </si>
   <si>
     <t>Central Friant WB</t>
+  </si>
+  <si>
+    <t>Historical validaton 1995-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28-year simulation using historical data and infrastructure </t>
+  </si>
+  <si>
+    <t>CDEC_1995_2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1820,6 +1829,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1931,7 +1946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1945,6 +1960,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2225,22 +2241,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.19921875" customWidth="1"/>
-    <col min="2" max="2" width="46.1328125" customWidth="1"/>
-    <col min="4" max="4" width="17.86328125" customWidth="1"/>
+    <col min="1" max="1" width="36.1796875" customWidth="1"/>
+    <col min="2" max="2" width="46.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="17.19921875" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>339</v>
       </c>
@@ -2260,16 +2276,14 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>334</v>
+        <v>586</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
-      </c>
-      <c r="C2">
-        <v>11</v>
-      </c>
+        <v>587</v>
+      </c>
+      <c r="C2" s="13"/>
       <c r="D2" t="s">
         <v>323</v>
       </c>
@@ -2277,21 +2291,21 @@
         <v>324</v>
       </c>
       <c r="F2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C3">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E3" t="s">
         <v>324</v>
@@ -2300,15 +2314,15 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="B4" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
         <v>326</v>
@@ -2317,55 +2331,55 @@
         <v>324</v>
       </c>
       <c r="F4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>326</v>
       </c>
       <c r="E5" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="F5" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B6" t="s">
-        <v>523</v>
+        <v>342</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>326</v>
       </c>
       <c r="E6" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>495</v>
+        <v>337</v>
       </c>
       <c r="B7" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -2377,32 +2391,32 @@
         <v>330</v>
       </c>
       <c r="F7" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>525</v>
+        <v>495</v>
       </c>
       <c r="B8" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C8">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>326</v>
       </c>
       <c r="E8" t="s">
-        <v>527</v>
+        <v>330</v>
       </c>
       <c r="F8" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B9" t="s">
         <v>526</v>
@@ -2417,12 +2431,12 @@
         <v>527</v>
       </c>
       <c r="F9" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B10" t="s">
         <v>526</v>
@@ -2437,12 +2451,12 @@
         <v>527</v>
       </c>
       <c r="F10" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B11" t="s">
         <v>526</v>
@@ -2457,12 +2471,12 @@
         <v>527</v>
       </c>
       <c r="F11" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B12" t="s">
         <v>526</v>
@@ -2477,12 +2491,12 @@
         <v>527</v>
       </c>
       <c r="F12" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B13" t="s">
         <v>526</v>
@@ -2497,12 +2511,12 @@
         <v>527</v>
       </c>
       <c r="F13" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B14" t="s">
         <v>526</v>
@@ -2517,12 +2531,12 @@
         <v>527</v>
       </c>
       <c r="F14" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B15" t="s">
         <v>526</v>
@@ -2537,12 +2551,12 @@
         <v>527</v>
       </c>
       <c r="F15" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B16" t="s">
         <v>526</v>
@@ -2557,12 +2571,12 @@
         <v>527</v>
       </c>
       <c r="F16" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B17" t="s">
         <v>526</v>
@@ -2577,12 +2591,12 @@
         <v>527</v>
       </c>
       <c r="F17" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B18" t="s">
         <v>526</v>
@@ -2597,12 +2611,12 @@
         <v>527</v>
       </c>
       <c r="F18" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B19" t="s">
         <v>526</v>
@@ -2617,12 +2631,12 @@
         <v>527</v>
       </c>
       <c r="F19" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B20" t="s">
         <v>526</v>
@@ -2637,12 +2651,12 @@
         <v>527</v>
       </c>
       <c r="F20" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B21" t="s">
         <v>526</v>
@@ -2657,12 +2671,12 @@
         <v>527</v>
       </c>
       <c r="F21" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B22" t="s">
         <v>526</v>
@@ -2677,12 +2691,12 @@
         <v>527</v>
       </c>
       <c r="F22" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B23" t="s">
         <v>526</v>
@@ -2697,12 +2711,12 @@
         <v>527</v>
       </c>
       <c r="F23" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B24" t="s">
         <v>526</v>
@@ -2717,12 +2731,12 @@
         <v>527</v>
       </c>
       <c r="F24" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B25" t="s">
         <v>526</v>
@@ -2737,12 +2751,12 @@
         <v>527</v>
       </c>
       <c r="F25" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B26" t="s">
         <v>526</v>
@@ -2757,12 +2771,12 @@
         <v>527</v>
       </c>
       <c r="F26" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B27" t="s">
         <v>526</v>
@@ -2777,12 +2791,12 @@
         <v>527</v>
       </c>
       <c r="F27" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B28" t="s">
         <v>526</v>
@@ -2797,12 +2811,12 @@
         <v>527</v>
       </c>
       <c r="F28" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B29" t="s">
         <v>526</v>
@@ -2817,10 +2831,31 @@
         <v>527</v>
       </c>
       <c r="F29" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>569</v>
+      </c>
+      <c r="B30" t="s">
+        <v>526</v>
+      </c>
+      <c r="C30">
+        <v>76</v>
+      </c>
+      <c r="D30" t="s">
+        <v>326</v>
+      </c>
+      <c r="E30" t="s">
+        <v>527</v>
+      </c>
+      <c r="F30" t="s">
         <v>570</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2834,15 +2869,15 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="20.1328125" customWidth="1"/>
-    <col min="5" max="5" width="38.19921875" customWidth="1"/>
+    <col min="3" max="3" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="38.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2853,7 +2888,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -2864,7 +2899,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -2875,7 +2910,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -2886,7 +2921,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -2897,7 +2932,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -2918,17 +2953,17 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="49.46484375" customWidth="1"/>
+    <col min="1" max="1" width="28.36328125" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.1328125" customWidth="1"/>
-    <col min="7" max="7" width="38.19921875" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="7" max="7" width="38.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -2945,7 +2980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>474</v>
       </c>
@@ -2962,7 +2997,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>475</v>
       </c>
@@ -2979,7 +3014,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>494</v>
       </c>
@@ -2996,7 +3031,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>476</v>
       </c>
@@ -3013,7 +3048,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>477</v>
       </c>
@@ -3030,7 +3065,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>478</v>
       </c>
@@ -3047,7 +3082,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>479</v>
       </c>
@@ -3064,7 +3099,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>480</v>
       </c>
@@ -3081,7 +3116,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>481</v>
       </c>
@@ -3098,7 +3133,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>482</v>
       </c>
@@ -3115,7 +3150,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>483</v>
       </c>
@@ -3132,7 +3167,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>484</v>
       </c>
@@ -3149,7 +3184,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>485</v>
       </c>
@@ -3166,7 +3201,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>486</v>
       </c>
@@ -3183,7 +3218,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>487</v>
       </c>
@@ -3200,7 +3235,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>488</v>
       </c>
@@ -3217,7 +3252,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>489</v>
       </c>
@@ -3234,7 +3269,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>490</v>
       </c>
@@ -3251,7 +3286,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>491</v>
       </c>
@@ -3268,7 +3303,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>492</v>
       </c>
@@ -3285,7 +3320,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>493</v>
       </c>
@@ -3315,15 +3350,15 @@
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.46484375" customWidth="1"/>
-    <col min="3" max="3" width="17.796875" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3334,7 +3369,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>468</v>
       </c>
@@ -3345,7 +3380,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>183</v>
       </c>
@@ -3356,7 +3391,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -3367,7 +3402,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>465</v>
       </c>
@@ -3378,7 +3413,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>462</v>
       </c>
@@ -3389,7 +3424,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -3400,7 +3435,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -3411,7 +3446,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>180</v>
       </c>
@@ -3422,7 +3457,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>456</v>
       </c>
@@ -3433,7 +3468,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>459</v>
       </c>
@@ -3444,7 +3479,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>184</v>
       </c>
@@ -3455,7 +3490,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>580</v>
       </c>
@@ -3466,7 +3501,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>583</v>
       </c>
@@ -3494,16 +3529,16 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.46484375" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.796875" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="1" max="2" width="14.36328125" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -3520,7 +3555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>473</v>
       </c>
@@ -3552,15 +3587,15 @@
       <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -3571,7 +3606,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3582,7 +3617,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -3593,7 +3628,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -3604,7 +3639,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -3615,7 +3650,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3626,7 +3661,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3637,7 +3672,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -3648,7 +3683,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -3659,7 +3694,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3670,7 +3705,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -3681,7 +3716,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -3692,7 +3727,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -3703,7 +3738,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -3714,7 +3749,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -3740,16 +3775,16 @@
       <selection pane="topRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.53125" customWidth="1"/>
-    <col min="2" max="2" width="30.19921875" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.796875" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -3766,7 +3801,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3783,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3800,7 +3835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3817,7 +3852,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3834,7 +3869,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -3851,7 +3886,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>279</v>
       </c>
@@ -3868,7 +3903,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>191</v>
       </c>
@@ -3885,7 +3920,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -3902,7 +3937,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3919,7 +3954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3936,7 +3971,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3953,7 +3988,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3970,7 +4005,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>367</v>
       </c>
@@ -3987,7 +4022,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>369</v>
       </c>
@@ -4018,14 +4053,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.46484375" customWidth="1"/>
-    <col min="2" max="2" width="12.86328125" customWidth="1"/>
-    <col min="3" max="3" width="19.19921875" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -4036,7 +4071,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -4047,7 +4082,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -4065,16 +4100,16 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.46484375" customWidth="1"/>
-    <col min="2" max="2" width="37.86328125" customWidth="1"/>
-    <col min="3" max="3" width="12.86328125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.19921875" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="37.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -4091,7 +4126,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>382</v>
       </c>
@@ -4108,7 +4143,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>381</v>
       </c>
@@ -4125,7 +4160,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>380</v>
       </c>
@@ -4142,7 +4177,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -4159,7 +4194,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -4176,7 +4211,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -4193,7 +4228,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -4210,7 +4245,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -4227,7 +4262,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -4245,7 +4280,7 @@
       </c>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -4262,7 +4297,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>267</v>
       </c>
@@ -4279,7 +4314,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>266</v>
       </c>
@@ -4296,7 +4331,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>268</v>
       </c>
@@ -4313,7 +4348,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -4330,7 +4365,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -4347,7 +4382,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>385</v>
       </c>
@@ -4381,14 +4416,14 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="20.86328125" customWidth="1"/>
-    <col min="4" max="4" width="13.796875" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -4402,7 +4437,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -4416,7 +4451,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -4430,7 +4465,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -4444,7 +4479,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -4458,7 +4493,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -4472,7 +4507,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -4486,7 +4521,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -4500,7 +4535,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -4514,7 +4549,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -4528,7 +4563,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -4542,7 +4577,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -4561,16 +4596,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="36.1328125" customWidth="1"/>
-    <col min="3" max="3" width="20.86328125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.796875" customWidth="1"/>
+    <col min="2" max="2" width="36.08984375" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
@@ -4587,7 +4622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -4604,7 +4639,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -4621,7 +4656,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -4638,7 +4673,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -4655,7 +4690,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -4672,7 +4707,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -4689,7 +4724,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>194</v>
       </c>
@@ -4715,21 +4750,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E24" sqref="E23:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.53125" customWidth="1"/>
-    <col min="4" max="4" width="9.796875" customWidth="1"/>
-    <col min="5" max="5" width="11.53125" customWidth="1"/>
-    <col min="6" max="6" width="8.796875" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -4740,7 +4775,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>164</v>
       </c>
@@ -4751,7 +4786,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -4762,7 +4797,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -4773,7 +4808,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -4784,7 +4819,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -4795,7 +4830,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -4806,7 +4841,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -4817,7 +4852,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -4828,7 +4863,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -4839,7 +4874,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -4850,7 +4885,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>163</v>
       </c>
@@ -4861,7 +4896,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>171</v>
       </c>
@@ -4872,7 +4907,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -4883,7 +4918,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -4894,7 +4929,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -4905,7 +4940,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -4916,7 +4951,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -4927,7 +4962,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -4938,7 +4973,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>167</v>
       </c>
@@ -4949,7 +4984,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -4960,7 +4995,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>103</v>
       </c>
@@ -4971,7 +5006,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -4982,7 +5017,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>165</v>
       </c>
@@ -4993,7 +5028,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -5004,7 +5039,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>125</v>
       </c>
@@ -5015,7 +5050,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>104</v>
       </c>
@@ -5026,7 +5061,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>126</v>
       </c>
@@ -5037,7 +5072,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -5048,7 +5083,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -5059,7 +5094,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>170</v>
       </c>
@@ -5070,7 +5105,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -5081,7 +5116,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>127</v>
       </c>
@@ -5092,7 +5127,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>105</v>
       </c>
@@ -5103,7 +5138,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -5114,7 +5149,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>128</v>
       </c>
@@ -5125,7 +5160,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -5136,7 +5171,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -5147,7 +5182,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>139</v>
       </c>
@@ -5158,7 +5193,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -5169,7 +5204,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>130</v>
       </c>
@@ -5180,7 +5215,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>131</v>
       </c>
@@ -5191,7 +5226,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -5202,7 +5237,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -5213,7 +5248,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>132</v>
       </c>
@@ -5224,7 +5259,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>133</v>
       </c>
@@ -5235,7 +5270,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>144</v>
       </c>
@@ -5246,7 +5281,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -5257,7 +5292,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -5268,7 +5303,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>113</v>
       </c>
@@ -5279,7 +5314,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>159</v>
       </c>
@@ -5290,7 +5325,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>152</v>
       </c>
@@ -5301,7 +5336,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>157</v>
       </c>
@@ -5312,7 +5347,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>151</v>
       </c>
@@ -5323,7 +5358,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>150</v>
       </c>
@@ -5334,7 +5369,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>160</v>
       </c>
@@ -5345,7 +5380,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>149</v>
       </c>
@@ -5372,19 +5407,19 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="55.53125" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.53125" customWidth="1"/>
-    <col min="6" max="6" width="9.796875" customWidth="1"/>
-    <col min="7" max="7" width="11.53125" customWidth="1"/>
-    <col min="8" max="8" width="8.796875" customWidth="1"/>
+    <col min="1" max="1" width="26.6328125" customWidth="1"/>
+    <col min="2" max="2" width="55.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -5401,7 +5436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>300</v>
       </c>
@@ -5418,7 +5453,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>301</v>
       </c>
@@ -5435,7 +5470,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>302</v>
       </c>
@@ -5452,7 +5487,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>303</v>
       </c>
@@ -5469,7 +5504,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>304</v>
       </c>
@@ -5486,7 +5521,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>306</v>
       </c>
@@ -5503,7 +5538,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>305</v>
       </c>
@@ -5520,7 +5555,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>440</v>
       </c>
@@ -5537,7 +5572,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>449</v>
       </c>
@@ -5554,7 +5589,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>473</v>
       </c>
@@ -5571,7 +5606,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>93</v>
       </c>
@@ -5588,7 +5623,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -5605,7 +5640,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -5622,7 +5657,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -5639,7 +5674,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -5656,7 +5691,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -5673,7 +5708,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -5690,7 +5725,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>187</v>
       </c>
@@ -5707,7 +5742,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>197</v>
       </c>
@@ -5724,7 +5759,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>199</v>
       </c>
@@ -5741,7 +5776,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>314</v>
       </c>

</xml_diff>

<commit_message>
update reservoir storage starting point
</commit_message>
<xml_diff>
--- a/gui_key.xlsx
+++ b/gui_key.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{916A722D-9717-4C37-899A-C1946F40FBF9}"/>
   <bookViews>
-    <workbookView xWindow="24420" yWindow="2460" windowWidth="23100" windowHeight="13524" tabRatio="727" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="32160" yWindow="4065" windowWidth="14400" windowHeight="8175" tabRatio="727" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_data" sheetId="7" r:id="rId1"/>
@@ -1971,6 +1971,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3578,7 +3582,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4090,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4744,7 +4748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix bug (daily input unit is af not cfs)
</commit_message>
<xml_diff>
--- a/gui_key.xlsx
+++ b/gui_key.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{916A722D-9717-4C37-899A-C1946F40FBF9}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="32160" yWindow="4065" windowWidth="14400" windowHeight="8175" tabRatio="727" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2500" yWindow="2500" windowWidth="14400" windowHeight="8170" tabRatio="727" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_data" sheetId="7" r:id="rId1"/>
@@ -3582,7 +3582,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A5" sqref="A5"/>
+      <selection pane="topRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3770,7 +3770,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D21" sqref="D21"/>
+      <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4094,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4591,7 +4591,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4748,7 +4748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -5404,8 +5404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>